<commit_message>
shoring up the organization
</commit_message>
<xml_diff>
--- a/data/raw_data/patient_log.xlsx
+++ b/data/raw_data/patient_log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAE259C-E6EE-442A-B9B7-5D2D53AC7E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096840AD-B3BA-495C-B712-091E3B40C5A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17920" yWindow="4860" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -149,9 +149,6 @@
     <t>06984</t>
   </si>
   <si>
-    <t>merged files without issue</t>
-  </si>
-  <si>
     <t>06988</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>LHC</t>
   </si>
   <si>
-    <t>Patient file split in two</t>
-  </si>
-  <si>
     <t>07106</t>
   </si>
   <si>
@@ -369,13 +363,28 @@
   </si>
   <si>
     <t>02/24/2020</t>
+  </si>
+  <si>
+    <t>07165</t>
+  </si>
+  <si>
+    <t>07169</t>
+  </si>
+  <si>
+    <t>07181</t>
+  </si>
+  <si>
+    <t>07140</t>
+  </si>
+  <si>
+    <t>Merged after split successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1232,25 +1241,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B36" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.125" customWidth="1"/>
-    <col min="5" max="5" width="19.125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08203125" customWidth="1"/>
+    <col min="5" max="5" width="19.08203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1321,22 +1330,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="46.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.65833333333333333</v>
-      </c>
+        <v>0.41111111111111115</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="G4" t="s">
         <v>11</v>
       </c>
@@ -1344,17 +1348,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>0.41111111111111115</v>
+        <v>0.47638888888888892</v>
       </c>
       <c r="E5" s="5"/>
+      <c r="F5" s="2">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
@@ -1362,19 +1369,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.47638888888888892</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.61319444444444449</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -1383,19 +1390,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.5083333333333333</v>
-      </c>
-      <c r="E7" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="2">
-        <v>0.61319444444444449</v>
+        <v>0.46388888888888885</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -1404,19 +1411,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.52361111111111114</v>
+      </c>
       <c r="F8" s="2">
-        <v>0.46388888888888885</v>
+        <v>0.39652777777777781</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -1425,61 +1431,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2">
-        <v>0.52361111111111114</v>
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F9" s="2">
-        <v>0.39652777777777781</v>
+        <v>0.64861111111111114</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="H9" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="46.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2">
-        <v>0.44791666666666669</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="F10" s="2">
-        <v>0.64861111111111114</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H10" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.38541666666666669</v>
+      <c r="D11" t="s">
+        <v>35</v>
       </c>
       <c r="F11" s="2">
-        <v>0.41250000000000003</v>
+        <v>0.44375000000000003</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -1488,18 +1494,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.49374999999999997</v>
       </c>
       <c r="F12" s="2">
-        <v>0.44375000000000003</v>
+        <v>0.53888888888888886</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -1508,18 +1514,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="2">
-        <v>0.49374999999999997</v>
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="F13" s="2">
-        <v>0.53888888888888886</v>
+        <v>0.57500000000000007</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -1528,21 +1537,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30.95">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>0.50972222222222219</v>
       </c>
       <c r="F14" s="2">
-        <v>0.57500000000000007</v>
+        <v>0.59236111111111112</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -1551,18 +1557,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="2">
-        <v>0.50972222222222219</v>
+        <v>0.5229166666666667</v>
       </c>
       <c r="F15" s="2">
-        <v>0.59236111111111112</v>
+        <v>0.65347222222222223</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -1571,18 +1577,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.5229166666666667</v>
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
       </c>
       <c r="F16" s="2">
-        <v>0.65347222222222223</v>
+        <v>0.50555555555555554</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -1591,18 +1597,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.41597222222222219</v>
       </c>
       <c r="F17" s="2">
-        <v>0.50555555555555554</v>
+        <v>0.44930555555555557</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -1611,18 +1617,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D18" s="2">
-        <v>0.41597222222222219</v>
+        <v>0.48819444444444443</v>
       </c>
       <c r="F18" s="2">
-        <v>0.44930555555555557</v>
+        <v>0.54236111111111118</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -1631,18 +1637,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="2">
-        <v>0.48819444444444443</v>
+        <v>0.44027777777777777</v>
       </c>
       <c r="F19" s="2">
-        <v>0.54236111111111118</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -1651,32 +1657,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="2">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.44027777777777777</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.4777777777777778</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D21" s="2">
         <v>0.34722222222222227</v>
@@ -1691,18 +1697,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D22" s="2">
-        <v>0.68611111111111101</v>
+        <v>0.43611111111111112</v>
       </c>
       <c r="F22" s="2">
-        <v>0.64583333333333337</v>
+        <v>0.73055555555555562</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
@@ -1711,18 +1717,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2">
-        <v>0.43611111111111112</v>
+        <v>0.39513888888888887</v>
       </c>
       <c r="F23" s="2">
-        <v>0.73055555555555562</v>
+        <v>0.49513888888888885</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1731,18 +1737,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.39513888888888887</v>
+        <v>58</v>
       </c>
       <c r="F24" s="2">
-        <v>0.49513888888888885</v>
+        <v>0.4680555555555555</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
@@ -1751,15 +1754,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F25" s="2">
-        <v>0.4680555555555555</v>
+        <v>0.58124999999999993</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
@@ -1768,15 +1771,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.39652777777777781</v>
       </c>
       <c r="F26" s="2">
-        <v>0.58124999999999993</v>
+        <v>0.53263888888888888</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
@@ -1785,18 +1791,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2">
-        <v>0.39652777777777781</v>
+        <v>0.40069444444444446</v>
       </c>
       <c r="F27" s="2">
-        <v>0.53263888888888888</v>
+        <v>0.47083333333333338</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -1805,18 +1811,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="D28" s="2">
-        <v>0.40069444444444446</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F28" s="2">
-        <v>0.47083333333333338</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
@@ -1825,18 +1831,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2">
-        <v>0.44444444444444442</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F29" s="2">
-        <v>0.51388888888888895</v>
+        <v>0.48680555555555555</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
@@ -1845,148 +1851,142 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="F30" s="2">
-        <v>0.48680555555555555</v>
-      </c>
-      <c r="G30" t="s">
-        <v>11</v>
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="H30" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="2">
-        <v>0.4145833333333333</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>69</v>
+        <v>0.63680555555555551</v>
       </c>
       <c r="F31" s="2">
-        <v>0.44166666666666665</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>0.6645833333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D32" s="2">
-        <v>0.63680555555555551</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0.6645833333333333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2">
-        <v>0.46527777777777773</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:9">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.50486111111111109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D34" s="2">
-        <v>0.47847222222222219</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="F34" s="2">
-        <v>0.50486111111111109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>0.37361111111111112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
       <c r="D35" s="2">
-        <v>0.43333333333333335</v>
+        <v>0.50069444444444444</v>
       </c>
       <c r="F35" s="2">
-        <v>0.37361111111111112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>0.5541666666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D36" s="2">
-        <v>0.50069444444444444</v>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="F36" s="2">
-        <v>0.5541666666666667</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30.95">
+        <v>0.62430555555555556</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" t="s">
-        <v>78</v>
+      <c r="C37" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D37" s="2">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>79</v>
+        <v>0.56111111111111112</v>
       </c>
       <c r="F37" s="2">
-        <v>0.62430555555555556</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B39" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.56111111111111112</v>
-      </c>
-      <c r="F38" s="2">
-        <v>0.6166666666666667</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="D39" s="2">
         <v>0.52083333333333337</v>
@@ -1998,18 +1998,18 @@
         <v>1</v>
       </c>
       <c r="I39" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D40" s="2">
         <v>0.4145833333333333</v>
@@ -2019,15 +2019,15 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="2">
         <v>0.46736111111111112</v>
@@ -2036,15 +2036,15 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D42" s="2">
         <v>0.4284722222222222</v>
@@ -2053,15 +2053,15 @@
         <v>0.57430555555555551</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D43" s="2">
         <v>0.5395833333333333</v>
@@ -2070,135 +2070,172 @@
         <v>0.59583333333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="2">
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D45" s="2">
         <v>0.55069444444444449</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D46" s="2">
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D47" s="2">
-        <v>0.60763888888888895</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>0.49444444444444446</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="1" t="s">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="2">
-        <v>0.49444444444444446</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="D49" s="2">
         <v>0.40972222222222227</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B52" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B53" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="1" t="s">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>112</v>
       </c>
     </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I57">
+    <sortCondition ref="A46"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>